<commit_message>
f/CashFlow:  Added npv scripts
</commit_message>
<xml_diff>
--- a/npv/src/blx_data.xlsx
+++ b/npv/src/blx_data.xlsx
@@ -11,7 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -92,11 +99,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -131,42 +141,50 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
         <v>43466.0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B2" s="3">
         <v>-5000.0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3">
+    <row r="3">
+      <c r="A3" s="4">
         <v>43831.0</v>
       </c>
-      <c r="B2" s="4">
-        <v>1000.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>44197.0</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>1000.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
-        <v>44562.0</v>
+      <c r="A4" s="4">
+        <v>44197.0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>1000.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
+        <v>44562.0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
         <v>44927.0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="5">
         <v>4000.0</v>
       </c>
     </row>

</xml_diff>